<commit_message>
updated expectations to use 99% confidence interval
+ updated gitingore to include maven files/ folders
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC7C3E4A-12FA-43BE-A968-DAEAD46CC8DC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{312ECF17-81F3-4D1E-8FC3-4D4FC4474AC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>Chance</t>
   </si>
   <si>
-    <t>1m runs error margin</t>
-  </si>
-  <si>
-    <t>95% confidence level</t>
-  </si>
-  <si>
     <t>Symbols</t>
   </si>
   <si>
@@ -81,15 +75,23 @@
   </si>
   <si>
     <t>2 x ACE</t>
+  </si>
+  <si>
+    <t>100k runs error margin</t>
+  </si>
+  <si>
+    <t>99% confidence level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -297,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -379,6 +381,24 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,24 +417,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,28 +703,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD3AD2D-3434-41F3-84D8-191D3A618518}">
-  <dimension ref="B1:D7"/>
+  <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="29" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -724,52 +733,115 @@
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="6">
         <v>0.4</v>
       </c>
-      <c r="D4" s="6">
-        <v>2.4004999479275146E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="24">
+        <v>3.9969188132860543E-3</v>
+      </c>
+      <c r="F4">
+        <f>SQRT(100000 * C4 * (1-C4)) * 2.58</f>
+        <v>399.6918813286054</v>
+      </c>
+      <c r="G4">
+        <f>F4/100000</f>
+        <v>3.9969188132860543E-3</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="6">
         <v>0.3</v>
       </c>
-      <c r="D5" s="6">
-        <v>2.9939494540378157E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="24">
+        <v>3.7387752005168754E-3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F7" si="0">SQRT(100000 * C5 * (1-C5)) * 2.58</f>
+        <v>373.87752005168755</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G7" si="1">F5/100000</f>
+        <v>3.7387752005168754E-3</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="6">
         <v>0.2</v>
       </c>
-      <c r="D6" s="6">
-        <v>3.9199999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="24">
+        <v>3.2634705452937677E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>326.34705452937675</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>3.2634705452937677E-3</v>
+      </c>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>3</v>
       </c>
       <c r="C7" s="7">
         <v>0.1</v>
       </c>
-      <c r="D7" s="7">
-        <v>5.8799999999999998E-3</v>
-      </c>
+      <c r="D7" s="25">
+        <v>2.4476029089703253E-3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>244.76029089703255</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2.4476029089703253E-3</v>
+      </c>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -785,35 +857,35 @@
   <dimension ref="B1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="E2" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="I2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="I2" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="30"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -832,16 +904,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -861,17 +933,17 @@
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="36">
+      <c r="I4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="30">
         <v>15</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="31">
         <v>4.6296296296296294E-3</v>
       </c>
-      <c r="L4" s="40">
-        <v>1.3305204382076737E-4</v>
+      <c r="L4" s="34">
+        <v>5.5384110459210452E-4</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -892,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J5" s="11">
         <v>14</v>
@@ -901,7 +973,7 @@
         <v>1.0973936899862825E-2</v>
       </c>
       <c r="L5" s="27">
-        <v>2.0419315001510646E-4</v>
+        <v>8.499723604911371E-4</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -922,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J6" s="11">
         <v>13</v>
@@ -931,7 +1003,7 @@
         <v>2.1433470507544586E-2</v>
       </c>
       <c r="L6" s="27">
-        <v>2.8385562109146083E-4</v>
+        <v>1.1815745644745545E-3</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -948,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J7" s="11">
         <v>12</v>
@@ -957,7 +1029,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="L7" s="27">
-        <v>3.7015104617192066E-4</v>
+        <v>1.5407870363415006E-3</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -973,17 +1045,17 @@
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="39">
+      <c r="I8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="33">
         <v>11</v>
       </c>
       <c r="K8" s="25">
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="L8" s="28">
-        <v>4.9824847537135184E-4</v>
+        <v>2.0740041117499153E-3</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -1027,6 +1099,14 @@
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="K11">
+        <f>SQRT(100000*K4*(1-K4))*2.58</f>
+        <v>55.384110459210454</v>
+      </c>
+      <c r="L11">
+        <f>K11/100000</f>
+        <v>5.5384110459210452E-4</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D12" s="23">
@@ -1041,6 +1121,14 @@
       <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="K12">
+        <f t="shared" ref="K12:K16" si="0">SQRT(100000*K5*(1-K5))*2.58</f>
+        <v>84.99723604911371</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12:L15" si="1">K12/100000</f>
+        <v>8.499723604911371E-4</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D13" s="23">
@@ -1055,6 +1143,14 @@
       <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>118.15745644745544</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>1.1815745644745545E-3</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D14" s="23">
@@ -1069,6 +1165,14 @@
       <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>154.07870363415006</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>1.5407870363415006E-3</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D15" s="23">
@@ -1082,6 +1186,14 @@
       </c>
       <c r="G15" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>207.40041117499155</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>2.0740041117499153E-3</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
removed calculations from excel
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{312ECF17-81F3-4D1E-8FC3-4D4FC4474AC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E0B3540-8ED0-4ADE-975D-8ED20D8C5DFC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,8 +90,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -399,6 +399,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,12 +423,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +706,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,10 +717,10 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="14" t="s">
         <v>19</v>
       </c>
@@ -746,16 +746,8 @@
       <c r="D4" s="24">
         <v>3.9969188132860543E-3</v>
       </c>
-      <c r="F4">
-        <f>SQRT(100000 * C4 * (1-C4)) * 2.58</f>
-        <v>399.6918813286054</v>
-      </c>
-      <c r="G4">
-        <f>F4/100000</f>
-        <v>3.9969188132860543E-3</v>
-      </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -767,16 +759,8 @@
       <c r="D5" s="24">
         <v>3.7387752005168754E-3</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F7" si="0">SQRT(100000 * C5 * (1-C5)) * 2.58</f>
-        <v>373.87752005168755</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G7" si="1">F5/100000</f>
-        <v>3.7387752005168754E-3</v>
-      </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
@@ -788,16 +772,8 @@
       <c r="D6" s="24">
         <v>3.2634705452937677E-3</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>326.34705452937675</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>3.2634705452937677E-3</v>
-      </c>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
@@ -809,39 +785,31 @@
       <c r="D7" s="25">
         <v>2.4476029089703253E-3</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>244.76029089703255</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>2.4476029089703253E-3</v>
-      </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="36"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="36"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I14" s="41"/>
+      <c r="I14" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -857,7 +825,7 @@
   <dimension ref="B1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,16 +842,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="I2" s="35" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
+      <c r="I2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="36"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="40"/>
       <c r="L2" s="14" t="s">
         <v>19</v>
       </c>
@@ -1099,14 +1067,6 @@
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K11">
-        <f>SQRT(100000*K4*(1-K4))*2.58</f>
-        <v>55.384110459210454</v>
-      </c>
-      <c r="L11">
-        <f>K11/100000</f>
-        <v>5.5384110459210452E-4</v>
-      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D12" s="23">
@@ -1121,14 +1081,6 @@
       <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K12">
-        <f t="shared" ref="K12:K16" si="0">SQRT(100000*K5*(1-K5))*2.58</f>
-        <v>84.99723604911371</v>
-      </c>
-      <c r="L12">
-        <f t="shared" ref="L12:L15" si="1">K12/100000</f>
-        <v>8.499723604911371E-4</v>
-      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D13" s="23">
@@ -1143,14 +1095,6 @@
       <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>118.15745644745544</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>1.1815745644745545E-3</v>
-      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D14" s="23">
@@ -1165,14 +1109,6 @@
       <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>154.07870363415006</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>1.5407870363415006E-3</v>
-      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D15" s="23">
@@ -1186,14 +1122,6 @@
       </c>
       <c r="G15" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>207.40041117499155</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
-        <v>2.0740041117499153E-3</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>